<commit_message>
Temporal clones replaced by InterfaceVariables
</commit_message>
<xml_diff>
--- a/IDA2015/PreliminaryExperiments/WasteIncineratorMoutParametersVMP_MLfading.xlsx
+++ b/IDA2015/PreliminaryExperiments/WasteIncineratorMoutParametersVMP_MLfading.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9800" yWindow="60" windowWidth="16000" windowHeight="13140" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16000" windowHeight="10500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -99,8 +99,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -115,13 +117,15 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -451,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1056,6 +1060,293 @@
       </c>
       <c r="J22">
         <v>1.9696449327366501E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24">
+        <f>B5-B15</f>
+        <v>0.70220797106452426</v>
+      </c>
+      <c r="C24">
+        <f t="shared" ref="C24:J24" si="0">C5-C15</f>
+        <v>-6.7657345547128989E-2</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>2.668450593240369E-2</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>3.7373322106100101E-2</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>2.6492756730800426E-3</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="0"/>
+        <v>-8.1752816153819914E-5</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="0"/>
+        <v>8.1002706873971403E-2</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="0"/>
+        <v>2.866402839359905E-3</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="0"/>
+        <v>-6.4945500156022998E-5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="B25">
+        <f t="shared" ref="B25:J30" si="1">B6-B16</f>
+        <v>3.2327362685137992</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="1"/>
+        <v>-0.23489063198839999</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="1"/>
+        <v>0.58922409918794416</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="1"/>
+        <v>2.0579552347478151E-2</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="1"/>
+        <v>-2.2172285859989316E-5</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="1"/>
+        <v>-1.1097921192043995E-4</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="1"/>
+        <v>3.6549240702470301E-2</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="1"/>
+        <v>3.1478792211601103E-3</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="1"/>
+        <v>-1.0759196662623195E-4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26">
+        <v>10</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="1"/>
+        <v>-1.483756019840959E-2</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="1"/>
+        <v>-7.8357421589902998E-5</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="1"/>
+        <v>4.7698495706000217E-6</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="1"/>
+        <v>1.1313973636044529E-2</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="1"/>
+        <v>-1.4212718425199444E-3</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="1"/>
+        <v>-3.9460279455590021E-5</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="1"/>
+        <v>1.3823205776761679E-2</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="1"/>
+        <v>-3.0312155396301499E-3</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="1"/>
+        <v>-5.0968068856400159E-5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27">
+        <v>50</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="1"/>
+        <v>-2.168410393776515E-2</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="1"/>
+        <v>-1.8090538749904184E-5</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="1"/>
+        <v>1.006080018438201E-4</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="1"/>
+        <v>-8.9450576219000932E-6</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="1"/>
+        <v>-2.2343289607995587E-4</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="1"/>
+        <v>-9.9608982117500335E-6</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="1"/>
+        <v>7.8368586200445699E-3</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="1"/>
+        <v>-4.494557939398458E-4</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="1"/>
+        <v>-1.1970268821349982E-5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28">
+        <v>100</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="1"/>
+        <v>-1.2422376143605024E-2</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="1"/>
+        <v>6.722049315999179E-5</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="1"/>
+        <v>1.3591619484620973E-4</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="1"/>
+        <v>-1.5685582591929608E-3</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="1"/>
+        <v>-2.3946194593404968E-4</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="1"/>
+        <v>-3.5376670461601326E-6</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="1"/>
+        <v>6.1623614237118493E-3</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="1"/>
+        <v>-6.07821462924929E-4</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="1"/>
+        <v>-3.1858636593798569E-6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29">
+        <v>1000</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="1"/>
+        <v>8.0379002340856488E-4</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="1"/>
+        <v>3.6095974120131658E-5</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="1"/>
+        <v>1.9911093717161999E-4</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="1"/>
+        <v>1.4170455985256008E-3</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="1"/>
+        <v>4.640908038999747E-5</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="1"/>
+        <v>1.2637952481500984E-4</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="1"/>
+        <v>2.2252994034583839E-3</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="1"/>
+        <v>7.3340358049955867E-5</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="1"/>
+        <v>6.697668556210996E-5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30">
+        <v>5000</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="1"/>
+        <v>9.6125594917321404E-4</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="1"/>
+        <v>-1.4515011459881322E-5</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="1"/>
+        <v>2.0961170103247963E-4</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="1"/>
+        <v>1.00732015653677E-3</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="1"/>
+        <v>-1.3074933050027937E-5</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="1"/>
+        <v>2.0002573875636982E-4</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="1"/>
+        <v>1.047393560990653E-3</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="1"/>
+        <v>-1.1570579319997165E-5</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="1"/>
+        <v>1.8823611480655016E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>